<commit_message>
Minor update and correction
</commit_message>
<xml_diff>
--- a/Other/Saved_Results_3_3_Riassunto.xlsx
+++ b/Other/Saved_Results_3_3_Riassunto.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\albi2\Documents\GitHub\Variational-Autoencoder-for-EEG-analysis\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE174443-AFE2-4B0F-8DF6-2E2D61B40253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D75CBF2E-FFD7-429A-BD71-B973AEF239BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="9" r:id="rId1"/>
+    <sheet name="Recon loss" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="19">
   <si>
     <t>AVG</t>
   </si>
@@ -75,11 +76,32 @@
   <si>
     <t>Hidden space dimension</t>
   </si>
+  <si>
+    <t>vEEGNet2</t>
+  </si>
+  <si>
+    <t>Train set</t>
+  </si>
+  <si>
+    <t>Test set</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>vEEGNet1</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -254,6 +276,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,12 +314,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -569,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA043637-3640-4DD5-9ECC-151F76986D87}">
   <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="R37" sqref="R37:U45"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,66 +612,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="22">
         <v>2</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="17">
+      <c r="C2" s="23"/>
+      <c r="D2" s="22">
         <v>4</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="23">
         <v>4</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="22">
         <v>8</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="23">
         <v>8</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="22">
         <v>16</v>
       </c>
-      <c r="I2" s="18">
+      <c r="I2" s="23">
         <v>16</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="22">
         <v>32</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="23">
         <v>32</v>
       </c>
-      <c r="L2" s="17">
+      <c r="L2" s="22">
         <v>64</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="23">
         <v>64</v>
       </c>
-      <c r="N2" s="17">
+      <c r="N2" s="22">
         <v>128</v>
       </c>
-      <c r="O2" s="18">
+      <c r="O2" s="23">
         <v>128</v>
       </c>
     </row>
@@ -648,44 +679,44 @@
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="24">
         <v>5220</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="19">
+      <c r="C3" s="25"/>
+      <c r="D3" s="24">
         <v>6760</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="25">
         <v>6760</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="24">
         <v>9840</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="25">
         <v>9840</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="24">
         <v>16000</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="25">
         <v>16000</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="24">
         <v>28320</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="25">
         <v>28320</v>
       </c>
-      <c r="L3" s="19">
+      <c r="L3" s="24">
         <v>52960</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="25">
         <v>52960</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="24">
         <v>102240</v>
       </c>
-      <c r="O3" s="20">
+      <c r="O3" s="25">
         <v>102240</v>
       </c>
     </row>
@@ -693,44 +724,44 @@
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="24">
         <v>580</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="19">
+      <c r="C4" s="25"/>
+      <c r="D4" s="24">
         <v>836</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="25">
         <v>836</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="24">
         <v>1348</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="25">
         <v>1348</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="24">
         <v>2372</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="25">
         <v>2372</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="24">
         <v>4420</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="25">
         <v>4420</v>
       </c>
-      <c r="L4" s="19">
+      <c r="L4" s="24">
         <v>8516</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="25">
         <v>8516</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="24">
         <v>16708</v>
       </c>
-      <c r="O4" s="20">
+      <c r="O4" s="25">
         <v>16708</v>
       </c>
     </row>
@@ -738,35 +769,35 @@
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="24">
         <f>SUM(B3:C4)</f>
         <v>5800</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="19">
+      <c r="C5" s="25"/>
+      <c r="D5" s="24">
         <v>7596</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="19">
+      <c r="E5" s="25"/>
+      <c r="F5" s="24">
         <v>11188</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="19">
+      <c r="G5" s="25"/>
+      <c r="H5" s="24">
         <v>18372</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="19">
+      <c r="I5" s="25"/>
+      <c r="J5" s="24">
         <v>32740</v>
       </c>
-      <c r="K5" s="20"/>
-      <c r="L5" s="19">
+      <c r="K5" s="25"/>
+      <c r="L5" s="24">
         <v>61476</v>
       </c>
-      <c r="M5" s="20"/>
-      <c r="N5" s="19">
+      <c r="M5" s="25"/>
+      <c r="N5" s="24">
         <v>118948</v>
       </c>
-      <c r="O5" s="20"/>
+      <c r="O5" s="25"/>
     </row>
     <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -1286,66 +1317,66 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="16"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="21"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="17">
+      <c r="B21" s="22">
         <v>2</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="17">
+      <c r="C21" s="23"/>
+      <c r="D21" s="22">
         <v>4</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="23">
         <v>4</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="22">
         <v>8</v>
       </c>
-      <c r="G21" s="18">
+      <c r="G21" s="23">
         <v>8</v>
       </c>
-      <c r="H21" s="17">
+      <c r="H21" s="22">
         <v>16</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="23">
         <v>16</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="22">
         <v>32</v>
       </c>
-      <c r="K21" s="18">
+      <c r="K21" s="23">
         <v>32</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="22">
         <v>64</v>
       </c>
-      <c r="M21" s="18">
+      <c r="M21" s="23">
         <v>64</v>
       </c>
-      <c r="N21" s="17">
+      <c r="N21" s="22">
         <v>128</v>
       </c>
-      <c r="O21" s="18">
+      <c r="O21" s="23">
         <v>128</v>
       </c>
     </row>
@@ -1353,44 +1384,44 @@
       <c r="A22" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="24">
         <v>5220</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="19">
+      <c r="C22" s="25"/>
+      <c r="D22" s="24">
         <v>6760</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="25">
         <v>6760</v>
       </c>
-      <c r="F22" s="19">
+      <c r="F22" s="24">
         <v>9840</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="25">
         <v>9840</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="24">
         <v>16000</v>
       </c>
-      <c r="I22" s="20">
+      <c r="I22" s="25">
         <v>16000</v>
       </c>
-      <c r="J22" s="19">
+      <c r="J22" s="24">
         <v>28320</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="25">
         <v>28320</v>
       </c>
-      <c r="L22" s="19">
+      <c r="L22" s="24">
         <v>52960</v>
       </c>
-      <c r="M22" s="20">
+      <c r="M22" s="25">
         <v>52960</v>
       </c>
-      <c r="N22" s="19">
+      <c r="N22" s="24">
         <v>102240</v>
       </c>
-      <c r="O22" s="20">
+      <c r="O22" s="25">
         <v>102240</v>
       </c>
     </row>
@@ -1398,44 +1429,44 @@
       <c r="A23" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="24">
         <v>580</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="19">
+      <c r="C23" s="25"/>
+      <c r="D23" s="24">
         <v>836</v>
       </c>
-      <c r="E23" s="20">
+      <c r="E23" s="25">
         <v>836</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="24">
         <v>1348</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="25">
         <v>1348</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="24">
         <v>2372</v>
       </c>
-      <c r="I23" s="20">
+      <c r="I23" s="25">
         <v>2372</v>
       </c>
-      <c r="J23" s="19">
+      <c r="J23" s="24">
         <v>4420</v>
       </c>
-      <c r="K23" s="20">
+      <c r="K23" s="25">
         <v>4420</v>
       </c>
-      <c r="L23" s="19">
+      <c r="L23" s="24">
         <v>8516</v>
       </c>
-      <c r="M23" s="20">
+      <c r="M23" s="25">
         <v>8516</v>
       </c>
-      <c r="N23" s="19">
+      <c r="N23" s="24">
         <v>16708</v>
       </c>
-      <c r="O23" s="20">
+      <c r="O23" s="25">
         <v>16708</v>
       </c>
     </row>
@@ -1443,35 +1474,35 @@
       <c r="A24" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="24">
         <f>SUM(B22:C23)</f>
         <v>5800</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="19">
+      <c r="C24" s="25"/>
+      <c r="D24" s="24">
         <v>7596</v>
       </c>
-      <c r="E24" s="20"/>
-      <c r="F24" s="19">
+      <c r="E24" s="25"/>
+      <c r="F24" s="24">
         <v>11188</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="19">
+      <c r="G24" s="25"/>
+      <c r="H24" s="24">
         <v>18372</v>
       </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="19">
+      <c r="I24" s="25"/>
+      <c r="J24" s="24">
         <v>32740</v>
       </c>
-      <c r="K24" s="20"/>
-      <c r="L24" s="19">
+      <c r="K24" s="25"/>
+      <c r="L24" s="24">
         <v>61476</v>
       </c>
-      <c r="M24" s="20"/>
-      <c r="N24" s="19">
+      <c r="M24" s="25"/>
+      <c r="N24" s="24">
         <v>118948</v>
       </c>
-      <c r="O24" s="20"/>
+      <c r="O24" s="25"/>
     </row>
     <row r="25" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
@@ -1951,137 +1982,137 @@
       <c r="O35" s="3"/>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="R37" s="21"/>
-      <c r="S37" s="22" t="s">
+      <c r="R37" s="14"/>
+      <c r="S37" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="T37" s="22"/>
-      <c r="U37" s="22"/>
+      <c r="T37" s="26"/>
+      <c r="U37" s="26"/>
     </row>
     <row r="38" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="R38" s="23" t="s">
+      <c r="R38" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="S38" s="24" t="s">
+      <c r="S38" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="T38" s="24" t="s">
+      <c r="T38" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="U38" s="24" t="s">
+      <c r="U38" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="R39" s="21">
+    <row r="39" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R39" s="14">
         <v>2</v>
       </c>
-      <c r="S39" s="21">
+      <c r="S39" s="14">
         <v>5220</v>
       </c>
-      <c r="T39" s="21">
+      <c r="T39" s="14">
         <v>580</v>
       </c>
-      <c r="U39" s="21">
+      <c r="U39" s="14">
         <f>S39+T39</f>
         <v>5800</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="R40" s="21">
+      <c r="R40" s="14">
         <v>4</v>
       </c>
-      <c r="S40" s="21">
+      <c r="S40" s="14">
         <v>6760</v>
       </c>
-      <c r="T40" s="21">
+      <c r="T40" s="14">
         <v>836</v>
       </c>
-      <c r="U40" s="21">
+      <c r="U40" s="14">
         <f t="shared" ref="U40:U45" si="0">S40+T40</f>
         <v>7596</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="R41" s="21">
+      <c r="R41" s="14">
         <v>8</v>
       </c>
-      <c r="S41" s="21">
+      <c r="S41" s="14">
         <v>9840</v>
       </c>
-      <c r="T41" s="21">
+      <c r="T41" s="14">
         <v>1348</v>
       </c>
-      <c r="U41" s="21">
+      <c r="U41" s="14">
         <f t="shared" si="0"/>
         <v>11188</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="R42" s="21">
+      <c r="R42" s="14">
         <v>16</v>
       </c>
-      <c r="S42" s="21">
+      <c r="S42" s="14">
         <v>16000</v>
       </c>
-      <c r="T42" s="21">
+      <c r="T42" s="14">
         <v>2372</v>
       </c>
-      <c r="U42" s="21">
+      <c r="U42" s="14">
         <f t="shared" si="0"/>
         <v>18372</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="R43" s="21">
+      <c r="R43" s="14">
         <v>32</v>
       </c>
-      <c r="S43" s="21">
+      <c r="S43" s="14">
         <v>28320</v>
       </c>
-      <c r="T43" s="21">
+      <c r="T43" s="14">
         <v>4420</v>
       </c>
-      <c r="U43" s="21">
+      <c r="U43" s="14">
         <f t="shared" si="0"/>
         <v>32740</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="R44" s="21">
+      <c r="R44" s="14">
         <v>64</v>
       </c>
-      <c r="S44" s="21">
+      <c r="S44" s="14">
         <v>52960</v>
       </c>
-      <c r="T44" s="21">
+      <c r="T44" s="14">
         <v>8516</v>
       </c>
-      <c r="U44" s="21">
+      <c r="U44" s="14">
         <f t="shared" si="0"/>
         <v>61476</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="R45" s="21">
+      <c r="R45" s="14">
         <v>128</v>
       </c>
-      <c r="S45" s="21">
+      <c r="S45" s="14">
         <v>102240</v>
       </c>
-      <c r="T45" s="21">
+      <c r="T45" s="14">
         <v>16708</v>
       </c>
-      <c r="U45" s="21">
+      <c r="U45" s="14">
         <f t="shared" si="0"/>
         <v>118948</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B58">
@@ -2197,4 +2228,424 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71862E18-3371-4D0C-B71E-FDEB48CE0BD5}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="7" width="8.88671875" style="16"/>
+    <col min="8" max="11" width="9.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B1" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="H1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="H2" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="27"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>1</v>
+      </c>
+      <c r="B4" s="17">
+        <v>27.819105148315401</v>
+      </c>
+      <c r="C4" s="17">
+        <v>5.7883524894714302</v>
+      </c>
+      <c r="D4" s="17">
+        <v>28.217075347900298</v>
+      </c>
+      <c r="E4" s="17">
+        <v>5.7505159378051696</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0.11243661493062899</v>
+      </c>
+      <c r="I4" s="18">
+        <v>1.30753712728619E-2</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0.114600673317909</v>
+      </c>
+      <c r="K4" s="18">
+        <v>1.2322624213993501E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>2</v>
+      </c>
+      <c r="B5" s="17">
+        <v>29.300304412841701</v>
+      </c>
+      <c r="C5" s="17">
+        <v>6.1959276199340803</v>
+      </c>
+      <c r="D5" s="17">
+        <v>66.131217956542898</v>
+      </c>
+      <c r="E5" s="17">
+        <v>54.884983062744098</v>
+      </c>
+      <c r="G5" s="16">
+        <v>2</v>
+      </c>
+      <c r="H5" s="18">
+        <v>0.111099272966384</v>
+      </c>
+      <c r="I5" s="18">
+        <v>1.5210096724331299E-2</v>
+      </c>
+      <c r="J5" s="18">
+        <v>0.117688655853271</v>
+      </c>
+      <c r="K5" s="18">
+        <v>1.51165537536144E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>3</v>
+      </c>
+      <c r="B6" s="17">
+        <v>50.161373138427699</v>
+      </c>
+      <c r="C6" s="17">
+        <v>15.3749685287475</v>
+      </c>
+      <c r="D6" s="17">
+        <v>47.550086975097599</v>
+      </c>
+      <c r="E6" s="17">
+        <v>13.700523376464799</v>
+      </c>
+      <c r="G6" s="16">
+        <v>3</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.113362155854702</v>
+      </c>
+      <c r="I6" s="18">
+        <v>1.5450110659003201E-2</v>
+      </c>
+      <c r="J6" s="18">
+        <v>0.117409385740756</v>
+      </c>
+      <c r="K6" s="18">
+        <v>1.4936817809939299E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>4</v>
+      </c>
+      <c r="B7" s="17">
+        <v>24.6262702941894</v>
+      </c>
+      <c r="C7" s="17">
+        <v>4.61799812316894</v>
+      </c>
+      <c r="D7" s="17">
+        <v>26.308483123779201</v>
+      </c>
+      <c r="E7" s="17">
+        <v>6.0111460685729901</v>
+      </c>
+      <c r="G7" s="16">
+        <v>4</v>
+      </c>
+      <c r="H7" s="18">
+        <v>0.111270301043987</v>
+      </c>
+      <c r="I7" s="18">
+        <v>1.27756791189312E-2</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0.110964998602867</v>
+      </c>
+      <c r="K7" s="18">
+        <v>1.25498119741678E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17">
+        <v>17.227256774902301</v>
+      </c>
+      <c r="C8" s="17">
+        <v>3.26134729385375</v>
+      </c>
+      <c r="D8" s="17">
+        <v>21.714687347412099</v>
+      </c>
+      <c r="E8" s="17">
+        <v>4.1025447845458896</v>
+      </c>
+      <c r="G8" s="16">
+        <v>5</v>
+      </c>
+      <c r="H8" s="18">
+        <v>9.7053796052932698E-2</v>
+      </c>
+      <c r="I8" s="18">
+        <v>1.56741999089717E-2</v>
+      </c>
+      <c r="J8" s="18">
+        <v>9.7031801939010606E-2</v>
+      </c>
+      <c r="K8" s="18">
+        <v>1.54026886448264E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>6</v>
+      </c>
+      <c r="B9" s="17">
+        <v>48.461551666259702</v>
+      </c>
+      <c r="C9" s="17">
+        <v>13.1246480941772</v>
+      </c>
+      <c r="D9" s="17">
+        <v>44.038581848144503</v>
+      </c>
+      <c r="E9" s="17">
+        <v>13.0730476379394</v>
+      </c>
+      <c r="G9" s="16">
+        <v>6</v>
+      </c>
+      <c r="H9" s="18">
+        <v>0.112158425152301</v>
+      </c>
+      <c r="I9" s="18">
+        <v>1.22668538242578E-2</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0.11236213147640201</v>
+      </c>
+      <c r="K9" s="18">
+        <v>1.32879987359046E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>7</v>
+      </c>
+      <c r="B10" s="17">
+        <v>22.328306198120099</v>
+      </c>
+      <c r="C10" s="17">
+        <v>4.6809668540954501</v>
+      </c>
+      <c r="D10" s="17">
+        <v>27.712659835815401</v>
+      </c>
+      <c r="E10" s="17">
+        <v>5.95298147201538</v>
+      </c>
+      <c r="G10" s="16">
+        <v>7</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0.10807297378778399</v>
+      </c>
+      <c r="I10" s="18">
+        <v>1.22585147619247E-2</v>
+      </c>
+      <c r="J10" s="18">
+        <v>0.107489600777626</v>
+      </c>
+      <c r="K10" s="18">
+        <v>1.2690768577158401E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>8</v>
+      </c>
+      <c r="B11" s="17">
+        <v>80.755172729492102</v>
+      </c>
+      <c r="C11" s="17">
+        <v>22.168025970458899</v>
+      </c>
+      <c r="D11" s="17">
+        <v>70.485687255859304</v>
+      </c>
+      <c r="E11" s="17">
+        <v>15.318737983703601</v>
+      </c>
+      <c r="G11" s="16">
+        <v>8</v>
+      </c>
+      <c r="H11" s="18">
+        <v>0.117369957268238</v>
+      </c>
+      <c r="I11" s="18">
+        <v>1.28288986161351E-2</v>
+      </c>
+      <c r="J11" s="18">
+        <v>0.115091055631637</v>
+      </c>
+      <c r="K11" s="18">
+        <v>1.1907119303941701E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>9</v>
+      </c>
+      <c r="B12" s="17">
+        <v>84.189361572265597</v>
+      </c>
+      <c r="C12" s="17">
+        <v>23.638046264648398</v>
+      </c>
+      <c r="D12" s="17">
+        <v>84.7215576171875</v>
+      </c>
+      <c r="E12" s="17">
+        <v>27.855247497558501</v>
+      </c>
+      <c r="G12" s="16">
+        <v>9</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0.118081644177436</v>
+      </c>
+      <c r="I12" s="18">
+        <v>1.4339622110128399E-2</v>
+      </c>
+      <c r="J12" s="18">
+        <v>0.12194769829511599</v>
+      </c>
+      <c r="K12" s="18">
+        <v>1.2967437505722001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="17">
+        <f>AVERAGE(B4:B12)</f>
+        <v>42.763189103868221</v>
+      </c>
+      <c r="C13" s="17">
+        <f t="shared" ref="C13:E13" si="0">AVERAGE(C4:C12)</f>
+        <v>10.983364582061737</v>
+      </c>
+      <c r="D13" s="17">
+        <f t="shared" si="0"/>
+        <v>46.320004145304317</v>
+      </c>
+      <c r="E13" s="17">
+        <f t="shared" si="0"/>
+        <v>16.294414202372202</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="18">
+        <f>AVERAGE(H4:H12)</f>
+        <v>0.11121168235937708</v>
+      </c>
+      <c r="I13" s="18">
+        <f t="shared" ref="I13" si="1">AVERAGE(I4:I12)</f>
+        <v>1.3764371888505033E-2</v>
+      </c>
+      <c r="J13" s="18">
+        <f t="shared" ref="J13" si="2">AVERAGE(J4:J12)</f>
+        <v>0.11273177795939941</v>
+      </c>
+      <c r="K13" s="18">
+        <f t="shared" ref="K13" si="3">AVERAGE(K4:K12)</f>
+        <v>1.3464646724363122E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>